<commit_message>
add grn import in pharmacy
</commit_message>
<xml_diff>
--- a/assets/template/grn_import.xlsx
+++ b/assets/template/grn_import.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>medicine</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Supplier</t>
+  </si>
+  <si>
+    <t>Po No</t>
   </si>
 </sst>
 </file>
@@ -396,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -413,7 +416,7 @@
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -432,11 +435,14 @@
       <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="E3" s="1"/>
     </row>
   </sheetData>

</xml_diff>